<commit_message>
hopefully finishing the final sweep
</commit_message>
<xml_diff>
--- a/rnaSample/rnaSample_J.PLAGGENBERG_06.07.19.xlsx
+++ b/rnaSample/rnaSample_J.PLAGGENBERG_06.07.19.xlsx
@@ -64,7 +64,7 @@
     <t xml:space="preserve">J.PLAGGENBERG</t>
   </si>
   <si>
-    <t xml:space="preserve">RiboPure0.25x</t>
+    <t xml:space="preserve">RiboPure0.25X</t>
   </si>
   <si>
     <t xml:space="preserve">NA</t>
@@ -234,7 +234,7 @@
   <dimension ref="A1:Z60"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2:H13"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -316,7 +316,8 @@
       <c r="G2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="5" t="b">
+      <c r="H2" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I2" s="6" t="n">
@@ -355,7 +356,8 @@
       <c r="G3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="5" t="b">
+      <c r="H3" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I3" s="6" t="n">
@@ -394,7 +396,8 @@
       <c r="G4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="5" t="b">
+      <c r="H4" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I4" s="6" t="n">
@@ -433,7 +436,8 @@
       <c r="G5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="5" t="b">
+      <c r="H5" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I5" s="6" t="n">
@@ -472,7 +476,8 @@
       <c r="G6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="5" t="b">
+      <c r="H6" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I6" s="6" t="n">
@@ -511,7 +516,8 @@
       <c r="G7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="5" t="b">
+      <c r="H7" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I7" s="6" t="n">
@@ -550,7 +556,8 @@
       <c r="G8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="5" t="b">
+      <c r="H8" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I8" s="6" t="n">
@@ -589,7 +596,8 @@
       <c r="G9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="5" t="b">
+      <c r="H9" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I9" s="6" t="n">
@@ -628,7 +636,8 @@
       <c r="G10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="5" t="b">
+      <c r="H10" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I10" s="6" t="n">
@@ -667,7 +676,8 @@
       <c r="G11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="5" t="b">
+      <c r="H11" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I11" s="6" t="n">
@@ -706,7 +716,8 @@
       <c r="G12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="5" t="b">
+      <c r="H12" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I12" s="6" t="n">
@@ -745,7 +756,8 @@
       <c r="G13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="5" t="b">
+      <c r="H13" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I13" s="6" t="n">

</xml_diff>